<commit_message>
add recommend by topic
</commit_message>
<xml_diff>
--- a/doc/Es搜索api接口_v2.xlsx
+++ b/doc/Es搜索api接口_v2.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="216">
   <si>
     <t>服务地址</t>
   </si>
@@ -5855,6 +5855,71 @@
   </si>
   <si>
     <t>0:否 1是</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>根据公司名或者新闻关键字推荐相关主题列表</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://54.222.222.172:8999/es/recommend/topics</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8999/es/recommend/topics</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST,GET</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>keyword</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>关键词</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>eg:"工商银行" 或者"雾霾"</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>num</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>推荐个数</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Int</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>默认为推荐&lt;=10个</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -6429,6 +6494,15 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6513,29 +6587,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -7834,10 +7899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F364"/>
+  <dimension ref="B2:F392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B232" workbookViewId="0">
-      <selection activeCell="F242" sqref="F242"/>
+    <sheetView tabSelected="1" topLeftCell="B346" workbookViewId="0">
+      <selection activeCell="D356" sqref="D356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -7850,113 +7915,113 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="78" customHeight="1">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
     </row>
     <row r="3" spans="2:6" ht="86.25" customHeight="1" thickBot="1">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
     </row>
     <row r="4" spans="2:6" ht="21" thickBot="1">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" spans="2:6" ht="13.5" thickBot="1">
       <c r="B5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="42"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="45"/>
     </row>
     <row r="6" spans="2:6" ht="13.5" thickBot="1">
       <c r="B6" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="45"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="48"/>
     </row>
     <row r="7" spans="2:6" ht="13.5" thickBot="1">
       <c r="B7" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="45"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="48"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51"/>
     </row>
     <row r="9" spans="2:6" ht="93.75" customHeight="1" thickBot="1">
       <c r="B9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
     </row>
     <row r="10" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B10" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="54"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="57"/>
     </row>
     <row r="11" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="54"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="57"/>
     </row>
     <row r="12" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B12" s="52"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="54"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="57"/>
     </row>
     <row r="13" spans="2:6" ht="13.5" thickBot="1">
       <c r="B13" s="7" t="s">
@@ -7998,18 +8063,18 @@
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B16" s="55"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
     </row>
     <row r="18" spans="2:6" ht="13.5" thickBot="1">
       <c r="B18" s="24" t="s">
@@ -8101,139 +8166,139 @@
       <c r="F24" s="26"/>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="32"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
     </row>
     <row r="26" spans="2:6">
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="38"/>
     </row>
     <row r="27" spans="2:6">
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="38"/>
     </row>
     <row r="28" spans="2:6">
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="2:6" ht="87.75" customHeight="1" thickBot="1">
-      <c r="B29" s="36"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="41"/>
     </row>
     <row r="30" spans="2:6" ht="46.5" customHeight="1" thickBot="1">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
     </row>
     <row r="31" spans="2:6" ht="21" customHeight="1" thickBot="1">
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
     </row>
     <row r="32" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B32" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="42"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="45"/>
     </row>
     <row r="33" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B33" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="42"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="45"/>
     </row>
     <row r="34" spans="2:6" ht="13.5" thickBot="1">
       <c r="B34" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="43" t="s">
+      <c r="C34" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="45"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="48"/>
     </row>
     <row r="35" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B35" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="46" t="s">
+      <c r="C35" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="48"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="51"/>
     </row>
     <row r="36" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
       <c r="B36" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="51"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="54"/>
     </row>
     <row r="37" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B37" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="52" t="s">
+      <c r="C37" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="54"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="57"/>
     </row>
     <row r="38" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B38" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="52" t="s">
+      <c r="C38" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="54"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="57"/>
     </row>
     <row r="39" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B39" s="52"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="54"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="57"/>
     </row>
     <row r="40" spans="2:6" ht="13.5" thickBot="1">
       <c r="B40" s="7" t="s">
@@ -8339,18 +8404,18 @@
       <c r="F48" s="9"/>
     </row>
     <row r="49" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B49" s="55"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="57"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="29"/>
     </row>
     <row r="50" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B50" s="27"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="29"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="32"/>
     </row>
     <row r="51" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B51" s="24" t="s">
@@ -8371,41 +8436,41 @@
       <c r="F52" s="26"/>
     </row>
     <row r="53" spans="2:6">
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="32"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="35"/>
     </row>
     <row r="54" spans="2:6">
-      <c r="B54" s="33"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="35"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="38"/>
     </row>
     <row r="55" spans="2:6">
-      <c r="B55" s="33"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="35"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="38"/>
     </row>
     <row r="56" spans="2:6">
-      <c r="B56" s="33"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="35"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="38"/>
     </row>
     <row r="57" spans="2:6" ht="12" customHeight="1" thickBot="1">
-      <c r="B57" s="36"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="38"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="41"/>
     </row>
     <row r="58" spans="2:6" ht="20.25" customHeight="1">
       <c r="B58" s="19"/>
@@ -8425,95 +8490,95 @@
       <c r="F60" s="16"/>
     </row>
     <row r="61" spans="2:6" ht="21" customHeight="1" thickBot="1">
-      <c r="B61" s="39" t="s">
+      <c r="B61" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="42"/>
     </row>
     <row r="62" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B62" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C62" s="40" t="s">
+      <c r="C62" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="41"/>
-      <c r="E62" s="41"/>
-      <c r="F62" s="42"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="45"/>
     </row>
     <row r="63" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B63" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="40" t="s">
+      <c r="C63" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D63" s="41"/>
-      <c r="E63" s="41"/>
-      <c r="F63" s="42"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="45"/>
     </row>
     <row r="64" spans="2:6" ht="13.5" thickBot="1">
       <c r="B64" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="43" t="s">
+      <c r="C64" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D64" s="44"/>
-      <c r="E64" s="44"/>
-      <c r="F64" s="45"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="48"/>
     </row>
     <row r="65" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B65" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="46" t="s">
+      <c r="C65" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="47"/>
-      <c r="E65" s="47"/>
-      <c r="F65" s="48"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="50"/>
+      <c r="F65" s="51"/>
     </row>
     <row r="66" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
       <c r="B66" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C66" s="49"/>
-      <c r="D66" s="50"/>
-      <c r="E66" s="50"/>
-      <c r="F66" s="51"/>
+      <c r="C66" s="52"/>
+      <c r="D66" s="53"/>
+      <c r="E66" s="53"/>
+      <c r="F66" s="54"/>
     </row>
     <row r="67" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B67" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C67" s="52" t="s">
+      <c r="C67" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D67" s="53"/>
-      <c r="E67" s="53"/>
-      <c r="F67" s="54"/>
+      <c r="D67" s="56"/>
+      <c r="E67" s="56"/>
+      <c r="F67" s="57"/>
     </row>
     <row r="68" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B68" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C68" s="52" t="s">
+      <c r="C68" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D68" s="53"/>
-      <c r="E68" s="53"/>
-      <c r="F68" s="54"/>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56"/>
+      <c r="F68" s="57"/>
     </row>
     <row r="69" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B69" s="52"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="53"/>
-      <c r="E69" s="53"/>
-      <c r="F69" s="54"/>
+      <c r="B69" s="55"/>
+      <c r="C69" s="56"/>
+      <c r="D69" s="56"/>
+      <c r="E69" s="56"/>
+      <c r="F69" s="57"/>
     </row>
     <row r="70" spans="2:6" ht="13.5" thickBot="1">
       <c r="B70" s="7" t="s">
@@ -8587,11 +8652,11 @@
       </c>
     </row>
     <row r="75" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B75" s="55"/>
-      <c r="C75" s="56"/>
-      <c r="D75" s="56"/>
-      <c r="E75" s="56"/>
-      <c r="F75" s="57"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="29"/>
     </row>
     <row r="76" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B76" s="24" t="s">
@@ -8686,38 +8751,38 @@
       <c r="B83" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="C83" s="31"/>
-      <c r="D83" s="31"/>
-      <c r="E83" s="31"/>
-      <c r="F83" s="32"/>
+      <c r="C83" s="34"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="34"/>
+      <c r="F83" s="35"/>
     </row>
     <row r="84" spans="2:6">
-      <c r="B84" s="33"/>
-      <c r="C84" s="34"/>
-      <c r="D84" s="34"/>
-      <c r="E84" s="34"/>
-      <c r="F84" s="35"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="38"/>
     </row>
     <row r="85" spans="2:6">
-      <c r="B85" s="33"/>
-      <c r="C85" s="34"/>
-      <c r="D85" s="34"/>
-      <c r="E85" s="34"/>
-      <c r="F85" s="35"/>
+      <c r="B85" s="36"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="38"/>
     </row>
     <row r="86" spans="2:6">
-      <c r="B86" s="33"/>
-      <c r="C86" s="34"/>
-      <c r="D86" s="34"/>
-      <c r="E86" s="34"/>
-      <c r="F86" s="35"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="38"/>
     </row>
     <row r="87" spans="2:6" ht="90" customHeight="1" thickBot="1">
-      <c r="B87" s="36"/>
-      <c r="C87" s="37"/>
-      <c r="D87" s="37"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="38"/>
+      <c r="B87" s="39"/>
+      <c r="C87" s="40"/>
+      <c r="D87" s="40"/>
+      <c r="E87" s="40"/>
+      <c r="F87" s="41"/>
     </row>
     <row r="88" spans="2:6" ht="20.25" customHeight="1">
       <c r="B88" s="19"/>
@@ -8737,95 +8802,95 @@
       <c r="F90" s="16"/>
     </row>
     <row r="91" spans="2:6" ht="21" customHeight="1" thickBot="1">
-      <c r="B91" s="39" t="s">
+      <c r="B91" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="C91" s="39"/>
-      <c r="D91" s="39"/>
-      <c r="E91" s="39"/>
-      <c r="F91" s="39"/>
+      <c r="C91" s="42"/>
+      <c r="D91" s="42"/>
+      <c r="E91" s="42"/>
+      <c r="F91" s="42"/>
     </row>
     <row r="92" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B92" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C92" s="40" t="s">
+      <c r="C92" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="D92" s="41"/>
-      <c r="E92" s="41"/>
-      <c r="F92" s="42"/>
+      <c r="D92" s="44"/>
+      <c r="E92" s="44"/>
+      <c r="F92" s="45"/>
     </row>
     <row r="93" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B93" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C93" s="40" t="s">
+      <c r="C93" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D93" s="41"/>
-      <c r="E93" s="41"/>
-      <c r="F93" s="42"/>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="45"/>
     </row>
     <row r="94" spans="2:6" ht="13.5" thickBot="1">
       <c r="B94" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C94" s="43" t="s">
+      <c r="C94" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D94" s="44"/>
-      <c r="E94" s="44"/>
-      <c r="F94" s="45"/>
+      <c r="D94" s="47"/>
+      <c r="E94" s="47"/>
+      <c r="F94" s="48"/>
     </row>
     <row r="95" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B95" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C95" s="46" t="s">
+      <c r="C95" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D95" s="47"/>
-      <c r="E95" s="47"/>
-      <c r="F95" s="48"/>
+      <c r="D95" s="50"/>
+      <c r="E95" s="50"/>
+      <c r="F95" s="51"/>
     </row>
     <row r="96" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
       <c r="B96" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C96" s="49"/>
-      <c r="D96" s="50"/>
-      <c r="E96" s="50"/>
-      <c r="F96" s="51"/>
+      <c r="C96" s="52"/>
+      <c r="D96" s="53"/>
+      <c r="E96" s="53"/>
+      <c r="F96" s="54"/>
     </row>
     <row r="97" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B97" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C97" s="52" t="s">
+      <c r="C97" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D97" s="53"/>
-      <c r="E97" s="53"/>
-      <c r="F97" s="54"/>
+      <c r="D97" s="56"/>
+      <c r="E97" s="56"/>
+      <c r="F97" s="57"/>
     </row>
     <row r="98" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B98" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C98" s="52" t="s">
+      <c r="C98" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D98" s="53"/>
-      <c r="E98" s="53"/>
-      <c r="F98" s="54"/>
+      <c r="D98" s="56"/>
+      <c r="E98" s="56"/>
+      <c r="F98" s="57"/>
     </row>
     <row r="99" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B99" s="52"/>
-      <c r="C99" s="53"/>
-      <c r="D99" s="53"/>
-      <c r="E99" s="53"/>
-      <c r="F99" s="54"/>
+      <c r="B99" s="55"/>
+      <c r="C99" s="56"/>
+      <c r="D99" s="56"/>
+      <c r="E99" s="56"/>
+      <c r="F99" s="57"/>
     </row>
     <row r="100" spans="2:6" ht="13.5" thickBot="1">
       <c r="B100" s="7" t="s">
@@ -8886,11 +8951,11 @@
       </c>
     </row>
     <row r="104" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B104" s="55"/>
-      <c r="C104" s="56"/>
-      <c r="D104" s="56"/>
-      <c r="E104" s="56"/>
-      <c r="F104" s="57"/>
+      <c r="B104" s="27"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="29"/>
     </row>
     <row r="105" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B105" s="24" t="s">
@@ -8980,41 +9045,41 @@
       <c r="F111" s="26"/>
     </row>
     <row r="112" spans="2:6">
-      <c r="B112" s="61" t="s">
+      <c r="B112" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="C112" s="31"/>
-      <c r="D112" s="31"/>
-      <c r="E112" s="31"/>
-      <c r="F112" s="32"/>
+      <c r="C112" s="34"/>
+      <c r="D112" s="34"/>
+      <c r="E112" s="34"/>
+      <c r="F112" s="35"/>
     </row>
     <row r="113" spans="2:6">
-      <c r="B113" s="33"/>
-      <c r="C113" s="34"/>
-      <c r="D113" s="34"/>
-      <c r="E113" s="34"/>
-      <c r="F113" s="35"/>
+      <c r="B113" s="36"/>
+      <c r="C113" s="37"/>
+      <c r="D113" s="37"/>
+      <c r="E113" s="37"/>
+      <c r="F113" s="38"/>
     </row>
     <row r="114" spans="2:6">
-      <c r="B114" s="33"/>
-      <c r="C114" s="34"/>
-      <c r="D114" s="34"/>
-      <c r="E114" s="34"/>
-      <c r="F114" s="35"/>
+      <c r="B114" s="36"/>
+      <c r="C114" s="37"/>
+      <c r="D114" s="37"/>
+      <c r="E114" s="37"/>
+      <c r="F114" s="38"/>
     </row>
     <row r="115" spans="2:6">
-      <c r="B115" s="33"/>
-      <c r="C115" s="34"/>
-      <c r="D115" s="34"/>
-      <c r="E115" s="34"/>
-      <c r="F115" s="35"/>
+      <c r="B115" s="36"/>
+      <c r="C115" s="37"/>
+      <c r="D115" s="37"/>
+      <c r="E115" s="37"/>
+      <c r="F115" s="38"/>
     </row>
     <row r="116" spans="2:6" ht="90" customHeight="1" thickBot="1">
-      <c r="B116" s="36"/>
-      <c r="C116" s="37"/>
-      <c r="D116" s="37"/>
-      <c r="E116" s="37"/>
-      <c r="F116" s="38"/>
+      <c r="B116" s="39"/>
+      <c r="C116" s="40"/>
+      <c r="D116" s="40"/>
+      <c r="E116" s="40"/>
+      <c r="F116" s="41"/>
     </row>
     <row r="117" spans="2:6" ht="20.25" customHeight="1">
       <c r="B117" s="19"/>
@@ -9034,95 +9099,95 @@
       <c r="F119" s="16"/>
     </row>
     <row r="120" spans="2:6" ht="21" customHeight="1" thickBot="1">
-      <c r="B120" s="39" t="s">
+      <c r="B120" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="C120" s="39"/>
-      <c r="D120" s="39"/>
-      <c r="E120" s="39"/>
-      <c r="F120" s="39"/>
+      <c r="C120" s="42"/>
+      <c r="D120" s="42"/>
+      <c r="E120" s="42"/>
+      <c r="F120" s="42"/>
     </row>
     <row r="121" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B121" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C121" s="40" t="s">
+      <c r="C121" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="D121" s="41"/>
-      <c r="E121" s="41"/>
-      <c r="F121" s="42"/>
+      <c r="D121" s="44"/>
+      <c r="E121" s="44"/>
+      <c r="F121" s="45"/>
     </row>
     <row r="122" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B122" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C122" s="40" t="s">
+      <c r="C122" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="D122" s="41"/>
-      <c r="E122" s="41"/>
-      <c r="F122" s="42"/>
+      <c r="D122" s="44"/>
+      <c r="E122" s="44"/>
+      <c r="F122" s="45"/>
     </row>
     <row r="123" spans="2:6" ht="13.5" thickBot="1">
       <c r="B123" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C123" s="43" t="s">
+      <c r="C123" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D123" s="44"/>
-      <c r="E123" s="44"/>
-      <c r="F123" s="45"/>
+      <c r="D123" s="47"/>
+      <c r="E123" s="47"/>
+      <c r="F123" s="48"/>
     </row>
     <row r="124" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B124" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C124" s="46" t="s">
+      <c r="C124" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D124" s="47"/>
-      <c r="E124" s="47"/>
-      <c r="F124" s="48"/>
+      <c r="D124" s="50"/>
+      <c r="E124" s="50"/>
+      <c r="F124" s="51"/>
     </row>
     <row r="125" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
       <c r="B125" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C125" s="49"/>
-      <c r="D125" s="50"/>
-      <c r="E125" s="50"/>
-      <c r="F125" s="51"/>
+      <c r="C125" s="52"/>
+      <c r="D125" s="53"/>
+      <c r="E125" s="53"/>
+      <c r="F125" s="54"/>
     </row>
     <row r="126" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B126" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C126" s="52" t="s">
+      <c r="C126" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D126" s="53"/>
-      <c r="E126" s="53"/>
-      <c r="F126" s="54"/>
+      <c r="D126" s="56"/>
+      <c r="E126" s="56"/>
+      <c r="F126" s="57"/>
     </row>
     <row r="127" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B127" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C127" s="52" t="s">
+      <c r="C127" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D127" s="53"/>
-      <c r="E127" s="53"/>
-      <c r="F127" s="54"/>
+      <c r="D127" s="56"/>
+      <c r="E127" s="56"/>
+      <c r="F127" s="57"/>
     </row>
     <row r="128" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B128" s="52"/>
-      <c r="C128" s="53"/>
-      <c r="D128" s="53"/>
-      <c r="E128" s="53"/>
-      <c r="F128" s="54"/>
+      <c r="B128" s="55"/>
+      <c r="C128" s="56"/>
+      <c r="D128" s="56"/>
+      <c r="E128" s="56"/>
+      <c r="F128" s="57"/>
     </row>
     <row r="129" spans="2:6" ht="13.5" thickBot="1">
       <c r="B129" s="7" t="s">
@@ -9149,11 +9214,11 @@
       <c r="F130" s="26"/>
     </row>
     <row r="131" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B131" s="55"/>
-      <c r="C131" s="56"/>
-      <c r="D131" s="56"/>
-      <c r="E131" s="56"/>
-      <c r="F131" s="57"/>
+      <c r="B131" s="27"/>
+      <c r="C131" s="28"/>
+      <c r="D131" s="28"/>
+      <c r="E131" s="28"/>
+      <c r="F131" s="29"/>
     </row>
     <row r="132" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B132" s="24" t="s">
@@ -9243,41 +9308,41 @@
       <c r="F138" s="26"/>
     </row>
     <row r="139" spans="2:6">
-      <c r="B139" s="61" t="s">
+      <c r="B139" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="C139" s="31"/>
-      <c r="D139" s="31"/>
-      <c r="E139" s="31"/>
-      <c r="F139" s="32"/>
+      <c r="C139" s="34"/>
+      <c r="D139" s="34"/>
+      <c r="E139" s="34"/>
+      <c r="F139" s="35"/>
     </row>
     <row r="140" spans="2:6">
-      <c r="B140" s="33"/>
-      <c r="C140" s="34"/>
-      <c r="D140" s="34"/>
-      <c r="E140" s="34"/>
-      <c r="F140" s="35"/>
+      <c r="B140" s="36"/>
+      <c r="C140" s="37"/>
+      <c r="D140" s="37"/>
+      <c r="E140" s="37"/>
+      <c r="F140" s="38"/>
     </row>
     <row r="141" spans="2:6">
-      <c r="B141" s="33"/>
-      <c r="C141" s="34"/>
-      <c r="D141" s="34"/>
-      <c r="E141" s="34"/>
-      <c r="F141" s="35"/>
+      <c r="B141" s="36"/>
+      <c r="C141" s="37"/>
+      <c r="D141" s="37"/>
+      <c r="E141" s="37"/>
+      <c r="F141" s="38"/>
     </row>
     <row r="142" spans="2:6">
-      <c r="B142" s="33"/>
-      <c r="C142" s="34"/>
-      <c r="D142" s="34"/>
-      <c r="E142" s="34"/>
-      <c r="F142" s="35"/>
+      <c r="B142" s="36"/>
+      <c r="C142" s="37"/>
+      <c r="D142" s="37"/>
+      <c r="E142" s="37"/>
+      <c r="F142" s="38"/>
     </row>
     <row r="143" spans="2:6" ht="90" customHeight="1" thickBot="1">
-      <c r="B143" s="36"/>
-      <c r="C143" s="37"/>
-      <c r="D143" s="37"/>
-      <c r="E143" s="37"/>
-      <c r="F143" s="38"/>
+      <c r="B143" s="39"/>
+      <c r="C143" s="40"/>
+      <c r="D143" s="40"/>
+      <c r="E143" s="40"/>
+      <c r="F143" s="41"/>
     </row>
     <row r="144" spans="2:6" ht="20.25" customHeight="1">
       <c r="B144" s="19"/>
@@ -9297,95 +9362,95 @@
       <c r="F146" s="16"/>
     </row>
     <row r="147" spans="2:6" ht="21" customHeight="1" thickBot="1">
-      <c r="B147" s="39" t="s">
+      <c r="B147" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="C147" s="39"/>
-      <c r="D147" s="39"/>
-      <c r="E147" s="39"/>
-      <c r="F147" s="39"/>
+      <c r="C147" s="42"/>
+      <c r="D147" s="42"/>
+      <c r="E147" s="42"/>
+      <c r="F147" s="42"/>
     </row>
     <row r="148" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B148" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C148" s="40" t="s">
+      <c r="C148" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="D148" s="41"/>
-      <c r="E148" s="41"/>
-      <c r="F148" s="42"/>
+      <c r="D148" s="44"/>
+      <c r="E148" s="44"/>
+      <c r="F148" s="45"/>
     </row>
     <row r="149" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B149" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C149" s="40" t="s">
+      <c r="C149" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="D149" s="41"/>
-      <c r="E149" s="41"/>
-      <c r="F149" s="42"/>
+      <c r="D149" s="44"/>
+      <c r="E149" s="44"/>
+      <c r="F149" s="45"/>
     </row>
     <row r="150" spans="2:6" ht="13.5" thickBot="1">
       <c r="B150" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C150" s="43" t="s">
+      <c r="C150" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D150" s="44"/>
-      <c r="E150" s="44"/>
-      <c r="F150" s="45"/>
+      <c r="D150" s="47"/>
+      <c r="E150" s="47"/>
+      <c r="F150" s="48"/>
     </row>
     <row r="151" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B151" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C151" s="46" t="s">
+      <c r="C151" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D151" s="47"/>
-      <c r="E151" s="47"/>
-      <c r="F151" s="48"/>
+      <c r="D151" s="50"/>
+      <c r="E151" s="50"/>
+      <c r="F151" s="51"/>
     </row>
     <row r="152" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
       <c r="B152" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C152" s="49"/>
-      <c r="D152" s="50"/>
-      <c r="E152" s="50"/>
-      <c r="F152" s="51"/>
+      <c r="C152" s="52"/>
+      <c r="D152" s="53"/>
+      <c r="E152" s="53"/>
+      <c r="F152" s="54"/>
     </row>
     <row r="153" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B153" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C153" s="52" t="s">
+      <c r="C153" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D153" s="53"/>
-      <c r="E153" s="53"/>
-      <c r="F153" s="54"/>
+      <c r="D153" s="56"/>
+      <c r="E153" s="56"/>
+      <c r="F153" s="57"/>
     </row>
     <row r="154" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B154" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C154" s="52" t="s">
+      <c r="C154" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D154" s="53"/>
-      <c r="E154" s="53"/>
-      <c r="F154" s="54"/>
+      <c r="D154" s="56"/>
+      <c r="E154" s="56"/>
+      <c r="F154" s="57"/>
     </row>
     <row r="155" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B155" s="52"/>
-      <c r="C155" s="53"/>
-      <c r="D155" s="53"/>
-      <c r="E155" s="53"/>
-      <c r="F155" s="54"/>
+      <c r="B155" s="55"/>
+      <c r="C155" s="56"/>
+      <c r="D155" s="56"/>
+      <c r="E155" s="56"/>
+      <c r="F155" s="57"/>
     </row>
     <row r="156" spans="2:6" ht="13.5" thickBot="1">
       <c r="B156" s="7" t="s">
@@ -9412,11 +9477,11 @@
       <c r="F157" s="26"/>
     </row>
     <row r="158" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B158" s="55"/>
-      <c r="C158" s="56"/>
-      <c r="D158" s="56"/>
-      <c r="E158" s="56"/>
-      <c r="F158" s="57"/>
+      <c r="B158" s="27"/>
+      <c r="C158" s="28"/>
+      <c r="D158" s="28"/>
+      <c r="E158" s="28"/>
+      <c r="F158" s="29"/>
     </row>
     <row r="159" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B159" s="24" t="s">
@@ -9506,41 +9571,41 @@
       <c r="F165" s="26"/>
     </row>
     <row r="166" spans="2:6">
-      <c r="B166" s="61" t="s">
+      <c r="B166" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="C166" s="31"/>
-      <c r="D166" s="31"/>
-      <c r="E166" s="31"/>
-      <c r="F166" s="32"/>
+      <c r="C166" s="34"/>
+      <c r="D166" s="34"/>
+      <c r="E166" s="34"/>
+      <c r="F166" s="35"/>
     </row>
     <row r="167" spans="2:6">
-      <c r="B167" s="33"/>
-      <c r="C167" s="34"/>
-      <c r="D167" s="34"/>
-      <c r="E167" s="34"/>
-      <c r="F167" s="35"/>
+      <c r="B167" s="36"/>
+      <c r="C167" s="37"/>
+      <c r="D167" s="37"/>
+      <c r="E167" s="37"/>
+      <c r="F167" s="38"/>
     </row>
     <row r="168" spans="2:6">
-      <c r="B168" s="33"/>
-      <c r="C168" s="34"/>
-      <c r="D168" s="34"/>
-      <c r="E168" s="34"/>
-      <c r="F168" s="35"/>
+      <c r="B168" s="36"/>
+      <c r="C168" s="37"/>
+      <c r="D168" s="37"/>
+      <c r="E168" s="37"/>
+      <c r="F168" s="38"/>
     </row>
     <row r="169" spans="2:6">
-      <c r="B169" s="33"/>
-      <c r="C169" s="34"/>
-      <c r="D169" s="34"/>
-      <c r="E169" s="34"/>
-      <c r="F169" s="35"/>
+      <c r="B169" s="36"/>
+      <c r="C169" s="37"/>
+      <c r="D169" s="37"/>
+      <c r="E169" s="37"/>
+      <c r="F169" s="38"/>
     </row>
     <row r="170" spans="2:6" ht="39" customHeight="1" thickBot="1">
-      <c r="B170" s="36"/>
-      <c r="C170" s="37"/>
-      <c r="D170" s="37"/>
-      <c r="E170" s="37"/>
-      <c r="F170" s="38"/>
+      <c r="B170" s="39"/>
+      <c r="C170" s="40"/>
+      <c r="D170" s="40"/>
+      <c r="E170" s="40"/>
+      <c r="F170" s="41"/>
     </row>
     <row r="171" spans="2:6" ht="39" customHeight="1" thickBot="1">
       <c r="B171" s="21"/>
@@ -9550,95 +9615,95 @@
       <c r="F171" s="21"/>
     </row>
     <row r="172" spans="2:6" ht="21" customHeight="1" thickBot="1">
-      <c r="B172" s="39" t="s">
+      <c r="B172" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="C172" s="39"/>
-      <c r="D172" s="39"/>
-      <c r="E172" s="39"/>
-      <c r="F172" s="39"/>
+      <c r="C172" s="42"/>
+      <c r="D172" s="42"/>
+      <c r="E172" s="42"/>
+      <c r="F172" s="42"/>
     </row>
     <row r="173" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B173" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C173" s="40" t="s">
+      <c r="C173" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="D173" s="41"/>
-      <c r="E173" s="41"/>
-      <c r="F173" s="42"/>
+      <c r="D173" s="44"/>
+      <c r="E173" s="44"/>
+      <c r="F173" s="45"/>
     </row>
     <row r="174" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B174" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C174" s="40" t="s">
+      <c r="C174" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="D174" s="41"/>
-      <c r="E174" s="41"/>
-      <c r="F174" s="42"/>
+      <c r="D174" s="44"/>
+      <c r="E174" s="44"/>
+      <c r="F174" s="45"/>
     </row>
     <row r="175" spans="2:6" ht="13.5" thickBot="1">
       <c r="B175" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C175" s="43" t="s">
+      <c r="C175" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D175" s="44"/>
-      <c r="E175" s="44"/>
-      <c r="F175" s="45"/>
+      <c r="D175" s="47"/>
+      <c r="E175" s="47"/>
+      <c r="F175" s="48"/>
     </row>
     <row r="176" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B176" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C176" s="46" t="s">
+      <c r="C176" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D176" s="47"/>
-      <c r="E176" s="47"/>
-      <c r="F176" s="48"/>
+      <c r="D176" s="50"/>
+      <c r="E176" s="50"/>
+      <c r="F176" s="51"/>
     </row>
     <row r="177" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
       <c r="B177" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C177" s="49"/>
-      <c r="D177" s="50"/>
-      <c r="E177" s="50"/>
-      <c r="F177" s="51"/>
+      <c r="C177" s="52"/>
+      <c r="D177" s="53"/>
+      <c r="E177" s="53"/>
+      <c r="F177" s="54"/>
     </row>
     <row r="178" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B178" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C178" s="52" t="s">
+      <c r="C178" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D178" s="53"/>
-      <c r="E178" s="53"/>
-      <c r="F178" s="54"/>
+      <c r="D178" s="56"/>
+      <c r="E178" s="56"/>
+      <c r="F178" s="57"/>
     </row>
     <row r="179" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B179" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C179" s="52" t="s">
+      <c r="C179" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D179" s="53"/>
-      <c r="E179" s="53"/>
-      <c r="F179" s="54"/>
+      <c r="D179" s="56"/>
+      <c r="E179" s="56"/>
+      <c r="F179" s="57"/>
     </row>
     <row r="180" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B180" s="52"/>
-      <c r="C180" s="53"/>
-      <c r="D180" s="53"/>
-      <c r="E180" s="53"/>
-      <c r="F180" s="54"/>
+      <c r="B180" s="55"/>
+      <c r="C180" s="56"/>
+      <c r="D180" s="56"/>
+      <c r="E180" s="56"/>
+      <c r="F180" s="57"/>
     </row>
     <row r="181" spans="2:6" ht="13.5" thickBot="1">
       <c r="B181" s="7" t="s">
@@ -9680,11 +9745,11 @@
       <c r="F183" s="9"/>
     </row>
     <row r="184" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B184" s="55"/>
-      <c r="C184" s="56"/>
-      <c r="D184" s="56"/>
-      <c r="E184" s="56"/>
-      <c r="F184" s="57"/>
+      <c r="B184" s="27"/>
+      <c r="C184" s="28"/>
+      <c r="D184" s="28"/>
+      <c r="E184" s="28"/>
+      <c r="F184" s="29"/>
     </row>
     <row r="185" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B185" s="24" t="s">
@@ -9774,41 +9839,41 @@
       <c r="F191" s="26"/>
     </row>
     <row r="192" spans="2:6">
-      <c r="B192" s="61" t="s">
+      <c r="B192" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="C192" s="31"/>
-      <c r="D192" s="31"/>
-      <c r="E192" s="31"/>
-      <c r="F192" s="32"/>
+      <c r="C192" s="34"/>
+      <c r="D192" s="34"/>
+      <c r="E192" s="34"/>
+      <c r="F192" s="35"/>
     </row>
     <row r="193" spans="2:6">
-      <c r="B193" s="33"/>
-      <c r="C193" s="34"/>
-      <c r="D193" s="34"/>
-      <c r="E193" s="34"/>
-      <c r="F193" s="35"/>
+      <c r="B193" s="36"/>
+      <c r="C193" s="37"/>
+      <c r="D193" s="37"/>
+      <c r="E193" s="37"/>
+      <c r="F193" s="38"/>
     </row>
     <row r="194" spans="2:6">
-      <c r="B194" s="33"/>
-      <c r="C194" s="34"/>
-      <c r="D194" s="34"/>
-      <c r="E194" s="34"/>
-      <c r="F194" s="35"/>
+      <c r="B194" s="36"/>
+      <c r="C194" s="37"/>
+      <c r="D194" s="37"/>
+      <c r="E194" s="37"/>
+      <c r="F194" s="38"/>
     </row>
     <row r="195" spans="2:6">
-      <c r="B195" s="33"/>
-      <c r="C195" s="34"/>
-      <c r="D195" s="34"/>
-      <c r="E195" s="34"/>
-      <c r="F195" s="35"/>
+      <c r="B195" s="36"/>
+      <c r="C195" s="37"/>
+      <c r="D195" s="37"/>
+      <c r="E195" s="37"/>
+      <c r="F195" s="38"/>
     </row>
     <row r="196" spans="2:6" ht="90" customHeight="1" thickBot="1">
-      <c r="B196" s="36"/>
-      <c r="C196" s="37"/>
-      <c r="D196" s="37"/>
-      <c r="E196" s="37"/>
-      <c r="F196" s="38"/>
+      <c r="B196" s="39"/>
+      <c r="C196" s="40"/>
+      <c r="D196" s="40"/>
+      <c r="E196" s="40"/>
+      <c r="F196" s="41"/>
     </row>
     <row r="197" spans="2:6" ht="90" customHeight="1" thickBot="1">
       <c r="B197" s="22"/>
@@ -9818,95 +9883,95 @@
       <c r="F197" s="22"/>
     </row>
     <row r="198" spans="2:6" ht="21" customHeight="1" thickBot="1">
-      <c r="B198" s="39" t="s">
+      <c r="B198" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="C198" s="39"/>
-      <c r="D198" s="39"/>
-      <c r="E198" s="39"/>
-      <c r="F198" s="39"/>
+      <c r="C198" s="42"/>
+      <c r="D198" s="42"/>
+      <c r="E198" s="42"/>
+      <c r="F198" s="42"/>
     </row>
     <row r="199" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B199" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C199" s="40" t="s">
+      <c r="C199" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="D199" s="41"/>
-      <c r="E199" s="41"/>
-      <c r="F199" s="42"/>
+      <c r="D199" s="44"/>
+      <c r="E199" s="44"/>
+      <c r="F199" s="45"/>
     </row>
     <row r="200" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B200" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C200" s="40" t="s">
+      <c r="C200" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="D200" s="41"/>
-      <c r="E200" s="41"/>
-      <c r="F200" s="42"/>
+      <c r="D200" s="44"/>
+      <c r="E200" s="44"/>
+      <c r="F200" s="45"/>
     </row>
     <row r="201" spans="2:6" ht="13.5" thickBot="1">
       <c r="B201" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C201" s="43" t="s">
+      <c r="C201" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D201" s="44"/>
-      <c r="E201" s="44"/>
-      <c r="F201" s="45"/>
+      <c r="D201" s="47"/>
+      <c r="E201" s="47"/>
+      <c r="F201" s="48"/>
     </row>
     <row r="202" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B202" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C202" s="46" t="s">
+      <c r="C202" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D202" s="47"/>
-      <c r="E202" s="47"/>
-      <c r="F202" s="48"/>
+      <c r="D202" s="50"/>
+      <c r="E202" s="50"/>
+      <c r="F202" s="51"/>
     </row>
     <row r="203" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
       <c r="B203" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C203" s="49"/>
-      <c r="D203" s="50"/>
-      <c r="E203" s="50"/>
-      <c r="F203" s="51"/>
+      <c r="C203" s="52"/>
+      <c r="D203" s="53"/>
+      <c r="E203" s="53"/>
+      <c r="F203" s="54"/>
     </row>
     <row r="204" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B204" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C204" s="52" t="s">
+      <c r="C204" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D204" s="53"/>
-      <c r="E204" s="53"/>
-      <c r="F204" s="54"/>
+      <c r="D204" s="56"/>
+      <c r="E204" s="56"/>
+      <c r="F204" s="57"/>
     </row>
     <row r="205" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B205" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C205" s="52" t="s">
+      <c r="C205" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D205" s="53"/>
-      <c r="E205" s="53"/>
-      <c r="F205" s="54"/>
+      <c r="D205" s="56"/>
+      <c r="E205" s="56"/>
+      <c r="F205" s="57"/>
     </row>
     <row r="206" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B206" s="52"/>
-      <c r="C206" s="53"/>
-      <c r="D206" s="53"/>
-      <c r="E206" s="53"/>
-      <c r="F206" s="54"/>
+      <c r="B206" s="55"/>
+      <c r="C206" s="56"/>
+      <c r="D206" s="56"/>
+      <c r="E206" s="56"/>
+      <c r="F206" s="57"/>
     </row>
     <row r="207" spans="2:6" ht="13.5" thickBot="1">
       <c r="B207" s="7" t="s">
@@ -9965,11 +10030,11 @@
       </c>
     </row>
     <row r="211" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B211" s="55"/>
-      <c r="C211" s="56"/>
-      <c r="D211" s="56"/>
-      <c r="E211" s="56"/>
-      <c r="F211" s="57"/>
+      <c r="B211" s="27"/>
+      <c r="C211" s="28"/>
+      <c r="D211" s="28"/>
+      <c r="E211" s="28"/>
+      <c r="F211" s="29"/>
     </row>
     <row r="212" spans="2:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B212" s="24" t="s">
@@ -10059,41 +10124,41 @@
       <c r="F218" s="26"/>
     </row>
     <row r="219" spans="2:6">
-      <c r="B219" s="61" t="s">
+      <c r="B219" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="C219" s="31"/>
-      <c r="D219" s="31"/>
-      <c r="E219" s="31"/>
-      <c r="F219" s="32"/>
+      <c r="C219" s="34"/>
+      <c r="D219" s="34"/>
+      <c r="E219" s="34"/>
+      <c r="F219" s="35"/>
     </row>
     <row r="220" spans="2:6">
-      <c r="B220" s="33"/>
-      <c r="C220" s="34"/>
-      <c r="D220" s="34"/>
-      <c r="E220" s="34"/>
-      <c r="F220" s="35"/>
+      <c r="B220" s="36"/>
+      <c r="C220" s="37"/>
+      <c r="D220" s="37"/>
+      <c r="E220" s="37"/>
+      <c r="F220" s="38"/>
     </row>
     <row r="221" spans="2:6">
-      <c r="B221" s="33"/>
-      <c r="C221" s="34"/>
-      <c r="D221" s="34"/>
-      <c r="E221" s="34"/>
-      <c r="F221" s="35"/>
+      <c r="B221" s="36"/>
+      <c r="C221" s="37"/>
+      <c r="D221" s="37"/>
+      <c r="E221" s="37"/>
+      <c r="F221" s="38"/>
     </row>
     <row r="222" spans="2:6">
-      <c r="B222" s="33"/>
-      <c r="C222" s="34"/>
-      <c r="D222" s="34"/>
-      <c r="E222" s="34"/>
-      <c r="F222" s="35"/>
+      <c r="B222" s="36"/>
+      <c r="C222" s="37"/>
+      <c r="D222" s="37"/>
+      <c r="E222" s="37"/>
+      <c r="F222" s="38"/>
     </row>
     <row r="223" spans="2:6" ht="90" customHeight="1" thickBot="1">
-      <c r="B223" s="36"/>
-      <c r="C223" s="37"/>
-      <c r="D223" s="37"/>
-      <c r="E223" s="37"/>
-      <c r="F223" s="38"/>
+      <c r="B223" s="39"/>
+      <c r="C223" s="40"/>
+      <c r="D223" s="40"/>
+      <c r="E223" s="40"/>
+      <c r="F223" s="41"/>
     </row>
     <row r="224" spans="2:6" ht="90" customHeight="1" thickBot="1">
       <c r="B224" s="23"/>
@@ -10103,95 +10168,95 @@
       <c r="F224" s="23"/>
     </row>
     <row r="225" spans="2:6" ht="21" thickBot="1">
-      <c r="B225" s="39" t="s">
+      <c r="B225" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="C225" s="39"/>
-      <c r="D225" s="39"/>
-      <c r="E225" s="39"/>
-      <c r="F225" s="39"/>
+      <c r="C225" s="42"/>
+      <c r="D225" s="42"/>
+      <c r="E225" s="42"/>
+      <c r="F225" s="42"/>
     </row>
     <row r="226" spans="2:6" ht="13.5" thickBot="1">
       <c r="B226" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C226" s="40" t="s">
+      <c r="C226" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="D226" s="41"/>
-      <c r="E226" s="41"/>
-      <c r="F226" s="42"/>
+      <c r="D226" s="44"/>
+      <c r="E226" s="44"/>
+      <c r="F226" s="45"/>
     </row>
     <row r="227" spans="2:6" ht="13.5" thickBot="1">
       <c r="B227" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C227" s="43" t="s">
+      <c r="C227" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="D227" s="44"/>
-      <c r="E227" s="44"/>
-      <c r="F227" s="45"/>
+      <c r="D227" s="47"/>
+      <c r="E227" s="47"/>
+      <c r="F227" s="48"/>
     </row>
     <row r="228" spans="2:6" ht="13.5" thickBot="1">
       <c r="B228" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C228" s="43" t="s">
+      <c r="C228" s="46" t="s">
         <v>175</v>
       </c>
-      <c r="D228" s="44"/>
-      <c r="E228" s="44"/>
-      <c r="F228" s="45"/>
+      <c r="D228" s="47"/>
+      <c r="E228" s="47"/>
+      <c r="F228" s="48"/>
     </row>
     <row r="229" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B229" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C229" s="46" t="s">
+      <c r="C229" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="D229" s="47"/>
-      <c r="E229" s="47"/>
-      <c r="F229" s="48"/>
+      <c r="D229" s="50"/>
+      <c r="E229" s="50"/>
+      <c r="F229" s="51"/>
     </row>
     <row r="230" spans="2:6" ht="93.75" customHeight="1" thickBot="1">
       <c r="B230" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C230" s="49"/>
-      <c r="D230" s="50"/>
-      <c r="E230" s="50"/>
-      <c r="F230" s="51"/>
+      <c r="C230" s="52"/>
+      <c r="D230" s="53"/>
+      <c r="E230" s="53"/>
+      <c r="F230" s="54"/>
     </row>
     <row r="231" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B231" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C231" s="52" t="s">
+      <c r="C231" s="55" t="s">
         <v>173</v>
       </c>
-      <c r="D231" s="53"/>
-      <c r="E231" s="53"/>
-      <c r="F231" s="54"/>
+      <c r="D231" s="56"/>
+      <c r="E231" s="56"/>
+      <c r="F231" s="57"/>
     </row>
     <row r="232" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B232" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C232" s="52" t="s">
+      <c r="C232" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D232" s="53"/>
-      <c r="E232" s="53"/>
-      <c r="F232" s="54"/>
+      <c r="D232" s="56"/>
+      <c r="E232" s="56"/>
+      <c r="F232" s="57"/>
     </row>
     <row r="233" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B233" s="52"/>
-      <c r="C233" s="53"/>
-      <c r="D233" s="53"/>
-      <c r="E233" s="53"/>
-      <c r="F233" s="54"/>
+      <c r="B233" s="55"/>
+      <c r="C233" s="56"/>
+      <c r="D233" s="56"/>
+      <c r="E233" s="56"/>
+      <c r="F233" s="57"/>
     </row>
     <row r="234" spans="2:6" ht="13.5" thickBot="1">
       <c r="B234" s="7" t="s">
@@ -10337,18 +10402,18 @@
       </c>
     </row>
     <row r="243" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B243" s="55"/>
-      <c r="C243" s="56"/>
-      <c r="D243" s="56"/>
-      <c r="E243" s="56"/>
-      <c r="F243" s="57"/>
+      <c r="B243" s="27"/>
+      <c r="C243" s="28"/>
+      <c r="D243" s="28"/>
+      <c r="E243" s="28"/>
+      <c r="F243" s="29"/>
     </row>
     <row r="244" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B244" s="27"/>
-      <c r="C244" s="28"/>
-      <c r="D244" s="28"/>
-      <c r="E244" s="28"/>
-      <c r="F244" s="29"/>
+      <c r="B244" s="30"/>
+      <c r="C244" s="31"/>
+      <c r="D244" s="31"/>
+      <c r="E244" s="31"/>
+      <c r="F244" s="32"/>
     </row>
     <row r="245" spans="2:6" ht="13.5" thickBot="1">
       <c r="B245" s="24" t="s">
@@ -10440,41 +10505,41 @@
       <c r="F251" s="26"/>
     </row>
     <row r="252" spans="2:6">
-      <c r="B252" s="30" t="s">
+      <c r="B252" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="C252" s="31"/>
-      <c r="D252" s="31"/>
-      <c r="E252" s="31"/>
-      <c r="F252" s="32"/>
+      <c r="C252" s="34"/>
+      <c r="D252" s="34"/>
+      <c r="E252" s="34"/>
+      <c r="F252" s="35"/>
     </row>
     <row r="253" spans="2:6">
-      <c r="B253" s="33"/>
-      <c r="C253" s="34"/>
-      <c r="D253" s="34"/>
-      <c r="E253" s="34"/>
-      <c r="F253" s="35"/>
+      <c r="B253" s="36"/>
+      <c r="C253" s="37"/>
+      <c r="D253" s="37"/>
+      <c r="E253" s="37"/>
+      <c r="F253" s="38"/>
     </row>
     <row r="254" spans="2:6">
-      <c r="B254" s="33"/>
-      <c r="C254" s="34"/>
-      <c r="D254" s="34"/>
-      <c r="E254" s="34"/>
-      <c r="F254" s="35"/>
+      <c r="B254" s="36"/>
+      <c r="C254" s="37"/>
+      <c r="D254" s="37"/>
+      <c r="E254" s="37"/>
+      <c r="F254" s="38"/>
     </row>
     <row r="255" spans="2:6">
-      <c r="B255" s="33"/>
-      <c r="C255" s="34"/>
-      <c r="D255" s="34"/>
-      <c r="E255" s="34"/>
-      <c r="F255" s="35"/>
+      <c r="B255" s="36"/>
+      <c r="C255" s="37"/>
+      <c r="D255" s="37"/>
+      <c r="E255" s="37"/>
+      <c r="F255" s="38"/>
     </row>
     <row r="256" spans="2:6" ht="145.5" customHeight="1" thickBot="1">
-      <c r="B256" s="36"/>
-      <c r="C256" s="37"/>
-      <c r="D256" s="37"/>
-      <c r="E256" s="37"/>
-      <c r="F256" s="38"/>
+      <c r="B256" s="39"/>
+      <c r="C256" s="40"/>
+      <c r="D256" s="40"/>
+      <c r="E256" s="40"/>
+      <c r="F256" s="41"/>
     </row>
     <row r="257" spans="2:6" ht="90" customHeight="1">
       <c r="B257" s="15"/>
@@ -10484,104 +10549,104 @@
       <c r="F257" s="15"/>
     </row>
     <row r="258" spans="2:6" ht="86.25" customHeight="1" thickBot="1">
-      <c r="B258" s="58" t="s">
+      <c r="B258" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C258" s="58"/>
-      <c r="D258" s="58"/>
-      <c r="E258" s="58"/>
-      <c r="F258" s="58"/>
+      <c r="C258" s="62"/>
+      <c r="D258" s="62"/>
+      <c r="E258" s="62"/>
+      <c r="F258" s="62"/>
     </row>
     <row r="259" spans="2:6" ht="21" thickBot="1">
-      <c r="B259" s="39" t="s">
+      <c r="B259" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C259" s="39"/>
-      <c r="D259" s="39"/>
-      <c r="E259" s="39"/>
-      <c r="F259" s="39"/>
+      <c r="C259" s="42"/>
+      <c r="D259" s="42"/>
+      <c r="E259" s="42"/>
+      <c r="F259" s="42"/>
     </row>
     <row r="260" spans="2:6" ht="13.5" thickBot="1">
       <c r="B260" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C260" s="40" t="s">
+      <c r="C260" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="D260" s="41"/>
-      <c r="E260" s="41"/>
-      <c r="F260" s="42"/>
+      <c r="D260" s="44"/>
+      <c r="E260" s="44"/>
+      <c r="F260" s="45"/>
     </row>
     <row r="261" spans="2:6" ht="13.5" thickBot="1">
       <c r="B261" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C261" s="40" t="s">
+      <c r="C261" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="D261" s="41"/>
-      <c r="E261" s="41"/>
-      <c r="F261" s="42"/>
+      <c r="D261" s="44"/>
+      <c r="E261" s="44"/>
+      <c r="F261" s="45"/>
     </row>
     <row r="262" spans="2:6" ht="13.5" thickBot="1">
       <c r="B262" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C262" s="43" t="s">
+      <c r="C262" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="D262" s="44"/>
-      <c r="E262" s="44"/>
-      <c r="F262" s="45"/>
+      <c r="D262" s="47"/>
+      <c r="E262" s="47"/>
+      <c r="F262" s="48"/>
     </row>
     <row r="263" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B263" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C263" s="46" t="s">
+      <c r="C263" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D263" s="47"/>
-      <c r="E263" s="47"/>
-      <c r="F263" s="48"/>
+      <c r="D263" s="50"/>
+      <c r="E263" s="50"/>
+      <c r="F263" s="51"/>
     </row>
     <row r="264" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
       <c r="B264" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C264" s="49"/>
-      <c r="D264" s="50"/>
-      <c r="E264" s="50"/>
-      <c r="F264" s="51"/>
+      <c r="C264" s="52"/>
+      <c r="D264" s="53"/>
+      <c r="E264" s="53"/>
+      <c r="F264" s="54"/>
     </row>
     <row r="265" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B265" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C265" s="52" t="s">
+      <c r="C265" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D265" s="53"/>
-      <c r="E265" s="53"/>
-      <c r="F265" s="54"/>
+      <c r="D265" s="56"/>
+      <c r="E265" s="56"/>
+      <c r="F265" s="57"/>
     </row>
     <row r="266" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B266" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C266" s="52" t="s">
+      <c r="C266" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D266" s="53"/>
-      <c r="E266" s="53"/>
-      <c r="F266" s="54"/>
+      <c r="D266" s="56"/>
+      <c r="E266" s="56"/>
+      <c r="F266" s="57"/>
     </row>
     <row r="267" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B267" s="52"/>
-      <c r="C267" s="53"/>
-      <c r="D267" s="53"/>
-      <c r="E267" s="53"/>
-      <c r="F267" s="54"/>
+      <c r="B267" s="55"/>
+      <c r="C267" s="56"/>
+      <c r="D267" s="56"/>
+      <c r="E267" s="56"/>
+      <c r="F267" s="57"/>
     </row>
     <row r="268" spans="2:6" ht="13.5" thickBot="1">
       <c r="B268" s="2" t="s">
@@ -10623,11 +10688,11 @@
       <c r="F270" s="3"/>
     </row>
     <row r="271" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B271" s="27"/>
-      <c r="C271" s="28"/>
-      <c r="D271" s="28"/>
-      <c r="E271" s="28"/>
-      <c r="F271" s="29"/>
+      <c r="B271" s="30"/>
+      <c r="C271" s="31"/>
+      <c r="D271" s="31"/>
+      <c r="E271" s="31"/>
+      <c r="F271" s="32"/>
     </row>
     <row r="272" spans="2:6" ht="13.5" thickBot="1">
       <c r="B272" s="24" t="s">
@@ -10717,133 +10782,133 @@
       <c r="F278" s="26"/>
     </row>
     <row r="279" spans="2:6">
-      <c r="B279" s="30" t="s">
+      <c r="B279" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C279" s="31"/>
-      <c r="D279" s="31"/>
-      <c r="E279" s="31"/>
-      <c r="F279" s="32"/>
+      <c r="C279" s="34"/>
+      <c r="D279" s="34"/>
+      <c r="E279" s="34"/>
+      <c r="F279" s="35"/>
     </row>
     <row r="280" spans="2:6">
-      <c r="B280" s="33"/>
-      <c r="C280" s="34"/>
-      <c r="D280" s="34"/>
-      <c r="E280" s="34"/>
-      <c r="F280" s="35"/>
+      <c r="B280" s="36"/>
+      <c r="C280" s="37"/>
+      <c r="D280" s="37"/>
+      <c r="E280" s="37"/>
+      <c r="F280" s="38"/>
     </row>
     <row r="281" spans="2:6">
-      <c r="B281" s="33"/>
-      <c r="C281" s="34"/>
-      <c r="D281" s="34"/>
-      <c r="E281" s="34"/>
-      <c r="F281" s="35"/>
+      <c r="B281" s="36"/>
+      <c r="C281" s="37"/>
+      <c r="D281" s="37"/>
+      <c r="E281" s="37"/>
+      <c r="F281" s="38"/>
     </row>
     <row r="282" spans="2:6">
-      <c r="B282" s="33"/>
-      <c r="C282" s="34"/>
-      <c r="D282" s="34"/>
-      <c r="E282" s="34"/>
-      <c r="F282" s="35"/>
+      <c r="B282" s="36"/>
+      <c r="C282" s="37"/>
+      <c r="D282" s="37"/>
+      <c r="E282" s="37"/>
+      <c r="F282" s="38"/>
     </row>
     <row r="283" spans="2:6" ht="87.75" customHeight="1" thickBot="1">
-      <c r="B283" s="36"/>
-      <c r="C283" s="37"/>
-      <c r="D283" s="37"/>
-      <c r="E283" s="37"/>
-      <c r="F283" s="38"/>
-    </row>
-    <row r="284" spans="2:6" s="62" customFormat="1" ht="29.25" customHeight="1" thickBot="1"/>
+      <c r="B283" s="39"/>
+      <c r="C283" s="40"/>
+      <c r="D283" s="40"/>
+      <c r="E283" s="40"/>
+      <c r="F283" s="41"/>
+    </row>
+    <row r="284" spans="2:6" s="59" customFormat="1" ht="29.25" customHeight="1" thickBot="1"/>
     <row r="285" spans="2:6" ht="21" thickBot="1">
-      <c r="B285" s="39" t="s">
+      <c r="B285" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C285" s="39"/>
-      <c r="D285" s="39"/>
-      <c r="E285" s="39"/>
-      <c r="F285" s="39"/>
+      <c r="C285" s="42"/>
+      <c r="D285" s="42"/>
+      <c r="E285" s="42"/>
+      <c r="F285" s="42"/>
     </row>
     <row r="286" spans="2:6" ht="13.5" thickBot="1">
       <c r="B286" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C286" s="40" t="s">
+      <c r="C286" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="D286" s="41"/>
-      <c r="E286" s="41"/>
-      <c r="F286" s="42"/>
+      <c r="D286" s="44"/>
+      <c r="E286" s="44"/>
+      <c r="F286" s="45"/>
     </row>
     <row r="287" spans="2:6" ht="13.5" thickBot="1">
       <c r="B287" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C287" s="40" t="s">
+      <c r="C287" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="D287" s="41"/>
-      <c r="E287" s="41"/>
-      <c r="F287" s="42"/>
+      <c r="D287" s="44"/>
+      <c r="E287" s="44"/>
+      <c r="F287" s="45"/>
     </row>
     <row r="288" spans="2:6" ht="13.5" thickBot="1">
       <c r="B288" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C288" s="43" t="s">
+      <c r="C288" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="D288" s="44"/>
-      <c r="E288" s="44"/>
-      <c r="F288" s="45"/>
+      <c r="D288" s="47"/>
+      <c r="E288" s="47"/>
+      <c r="F288" s="48"/>
     </row>
     <row r="289" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B289" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C289" s="46" t="s">
+      <c r="C289" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D289" s="47"/>
-      <c r="E289" s="47"/>
-      <c r="F289" s="48"/>
+      <c r="D289" s="50"/>
+      <c r="E289" s="50"/>
+      <c r="F289" s="51"/>
     </row>
     <row r="290" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
       <c r="B290" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C290" s="49"/>
-      <c r="D290" s="50"/>
-      <c r="E290" s="50"/>
-      <c r="F290" s="51"/>
+      <c r="C290" s="52"/>
+      <c r="D290" s="53"/>
+      <c r="E290" s="53"/>
+      <c r="F290" s="54"/>
     </row>
     <row r="291" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B291" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C291" s="52" t="s">
+      <c r="C291" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D291" s="53"/>
-      <c r="E291" s="53"/>
-      <c r="F291" s="54"/>
+      <c r="D291" s="56"/>
+      <c r="E291" s="56"/>
+      <c r="F291" s="57"/>
     </row>
     <row r="292" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B292" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C292" s="52" t="s">
+      <c r="C292" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D292" s="53"/>
-      <c r="E292" s="53"/>
-      <c r="F292" s="54"/>
+      <c r="D292" s="56"/>
+      <c r="E292" s="56"/>
+      <c r="F292" s="57"/>
     </row>
     <row r="293" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B293" s="52"/>
-      <c r="C293" s="53"/>
-      <c r="D293" s="53"/>
-      <c r="E293" s="53"/>
-      <c r="F293" s="54"/>
+      <c r="B293" s="55"/>
+      <c r="C293" s="56"/>
+      <c r="D293" s="56"/>
+      <c r="E293" s="56"/>
+      <c r="F293" s="57"/>
     </row>
     <row r="294" spans="2:6" ht="13.5" thickBot="1">
       <c r="B294" s="7" t="s">
@@ -10892,11 +10957,11 @@
       <c r="F297" s="9"/>
     </row>
     <row r="298" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B298" s="27"/>
-      <c r="C298" s="28"/>
-      <c r="D298" s="28"/>
-      <c r="E298" s="28"/>
-      <c r="F298" s="29"/>
+      <c r="B298" s="30"/>
+      <c r="C298" s="31"/>
+      <c r="D298" s="31"/>
+      <c r="E298" s="31"/>
+      <c r="F298" s="32"/>
     </row>
     <row r="299" spans="2:6" ht="13.5" thickBot="1">
       <c r="B299" s="24" t="s">
@@ -10986,134 +11051,134 @@
       <c r="F305" s="26"/>
     </row>
     <row r="306" spans="2:6">
-      <c r="B306" s="30" t="s">
+      <c r="B306" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="C306" s="31"/>
-      <c r="D306" s="31"/>
-      <c r="E306" s="31"/>
-      <c r="F306" s="32"/>
+      <c r="C306" s="34"/>
+      <c r="D306" s="34"/>
+      <c r="E306" s="34"/>
+      <c r="F306" s="35"/>
     </row>
     <row r="307" spans="2:6">
-      <c r="B307" s="33"/>
-      <c r="C307" s="34"/>
-      <c r="D307" s="34"/>
-      <c r="E307" s="34"/>
-      <c r="F307" s="35"/>
+      <c r="B307" s="36"/>
+      <c r="C307" s="37"/>
+      <c r="D307" s="37"/>
+      <c r="E307" s="37"/>
+      <c r="F307" s="38"/>
     </row>
     <row r="308" spans="2:6">
-      <c r="B308" s="33"/>
-      <c r="C308" s="34"/>
-      <c r="D308" s="34"/>
-      <c r="E308" s="34"/>
-      <c r="F308" s="35"/>
+      <c r="B308" s="36"/>
+      <c r="C308" s="37"/>
+      <c r="D308" s="37"/>
+      <c r="E308" s="37"/>
+      <c r="F308" s="38"/>
     </row>
     <row r="309" spans="2:6">
-      <c r="B309" s="33"/>
-      <c r="C309" s="34"/>
-      <c r="D309" s="34"/>
-      <c r="E309" s="34"/>
-      <c r="F309" s="35"/>
+      <c r="B309" s="36"/>
+      <c r="C309" s="37"/>
+      <c r="D309" s="37"/>
+      <c r="E309" s="37"/>
+      <c r="F309" s="38"/>
     </row>
     <row r="310" spans="2:6" ht="87.75" customHeight="1" thickBot="1">
-      <c r="B310" s="36"/>
-      <c r="C310" s="37"/>
-      <c r="D310" s="37"/>
-      <c r="E310" s="37"/>
-      <c r="F310" s="38"/>
+      <c r="B310" s="39"/>
+      <c r="C310" s="40"/>
+      <c r="D310" s="40"/>
+      <c r="E310" s="40"/>
+      <c r="F310" s="41"/>
     </row>
     <row r="311" spans="2:6" s="13" customFormat="1" ht="29.25" customHeight="1"/>
     <row r="312" spans="2:6" s="13" customFormat="1" ht="29.25" customHeight="1" thickBot="1"/>
     <row r="313" spans="2:6" ht="21" thickBot="1">
-      <c r="B313" s="39" t="s">
+      <c r="B313" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="C313" s="39"/>
-      <c r="D313" s="39"/>
-      <c r="E313" s="39"/>
-      <c r="F313" s="39"/>
+      <c r="C313" s="42"/>
+      <c r="D313" s="42"/>
+      <c r="E313" s="42"/>
+      <c r="F313" s="42"/>
     </row>
     <row r="314" spans="2:6" ht="13.5" thickBot="1">
       <c r="B314" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C314" s="40" t="s">
+      <c r="C314" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D314" s="41"/>
-      <c r="E314" s="41"/>
-      <c r="F314" s="42"/>
+      <c r="D314" s="44"/>
+      <c r="E314" s="44"/>
+      <c r="F314" s="45"/>
     </row>
     <row r="315" spans="2:6" ht="13.5" thickBot="1">
       <c r="B315" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C315" s="40" t="s">
+      <c r="C315" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="D315" s="41"/>
-      <c r="E315" s="41"/>
-      <c r="F315" s="42"/>
+      <c r="D315" s="44"/>
+      <c r="E315" s="44"/>
+      <c r="F315" s="45"/>
     </row>
     <row r="316" spans="2:6" ht="13.5" thickBot="1">
       <c r="B316" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C316" s="43" t="s">
+      <c r="C316" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="D316" s="44"/>
-      <c r="E316" s="44"/>
-      <c r="F316" s="45"/>
+      <c r="D316" s="47"/>
+      <c r="E316" s="47"/>
+      <c r="F316" s="48"/>
     </row>
     <row r="317" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B317" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C317" s="46" t="s">
+      <c r="C317" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D317" s="47"/>
-      <c r="E317" s="47"/>
-      <c r="F317" s="48"/>
+      <c r="D317" s="50"/>
+      <c r="E317" s="50"/>
+      <c r="F317" s="51"/>
     </row>
     <row r="318" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
       <c r="B318" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C318" s="49"/>
-      <c r="D318" s="50"/>
-      <c r="E318" s="50"/>
-      <c r="F318" s="51"/>
+      <c r="C318" s="52"/>
+      <c r="D318" s="53"/>
+      <c r="E318" s="53"/>
+      <c r="F318" s="54"/>
     </row>
     <row r="319" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B319" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C319" s="52" t="s">
+      <c r="C319" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D319" s="53"/>
-      <c r="E319" s="53"/>
-      <c r="F319" s="54"/>
+      <c r="D319" s="56"/>
+      <c r="E319" s="56"/>
+      <c r="F319" s="57"/>
     </row>
     <row r="320" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B320" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C320" s="52" t="s">
+      <c r="C320" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D320" s="53"/>
-      <c r="E320" s="53"/>
-      <c r="F320" s="54"/>
+      <c r="D320" s="56"/>
+      <c r="E320" s="56"/>
+      <c r="F320" s="57"/>
     </row>
     <row r="321" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B321" s="52"/>
-      <c r="C321" s="53"/>
-      <c r="D321" s="53"/>
-      <c r="E321" s="53"/>
-      <c r="F321" s="54"/>
+      <c r="B321" s="55"/>
+      <c r="C321" s="56"/>
+      <c r="D321" s="56"/>
+      <c r="E321" s="56"/>
+      <c r="F321" s="57"/>
     </row>
     <row r="322" spans="2:6" ht="13.5" thickBot="1">
       <c r="B322" s="7" t="s">
@@ -11155,11 +11220,11 @@
       <c r="F324" s="9"/>
     </row>
     <row r="325" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B325" s="27"/>
-      <c r="C325" s="28"/>
-      <c r="D325" s="28"/>
-      <c r="E325" s="28"/>
-      <c r="F325" s="29"/>
+      <c r="B325" s="30"/>
+      <c r="C325" s="31"/>
+      <c r="D325" s="31"/>
+      <c r="E325" s="31"/>
+      <c r="F325" s="32"/>
     </row>
     <row r="326" spans="2:6" ht="13.5" thickBot="1">
       <c r="B326" s="24" t="s">
@@ -11249,133 +11314,133 @@
       <c r="F332" s="26"/>
     </row>
     <row r="333" spans="2:6">
-      <c r="B333" s="30" t="s">
+      <c r="B333" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="C333" s="31"/>
-      <c r="D333" s="31"/>
-      <c r="E333" s="31"/>
-      <c r="F333" s="32"/>
+      <c r="C333" s="34"/>
+      <c r="D333" s="34"/>
+      <c r="E333" s="34"/>
+      <c r="F333" s="35"/>
     </row>
     <row r="334" spans="2:6">
-      <c r="B334" s="33"/>
-      <c r="C334" s="34"/>
-      <c r="D334" s="34"/>
-      <c r="E334" s="34"/>
-      <c r="F334" s="35"/>
+      <c r="B334" s="36"/>
+      <c r="C334" s="37"/>
+      <c r="D334" s="37"/>
+      <c r="E334" s="37"/>
+      <c r="F334" s="38"/>
     </row>
     <row r="335" spans="2:6">
-      <c r="B335" s="33"/>
-      <c r="C335" s="34"/>
-      <c r="D335" s="34"/>
-      <c r="E335" s="34"/>
-      <c r="F335" s="35"/>
+      <c r="B335" s="36"/>
+      <c r="C335" s="37"/>
+      <c r="D335" s="37"/>
+      <c r="E335" s="37"/>
+      <c r="F335" s="38"/>
     </row>
     <row r="336" spans="2:6">
-      <c r="B336" s="33"/>
-      <c r="C336" s="34"/>
-      <c r="D336" s="34"/>
-      <c r="E336" s="34"/>
-      <c r="F336" s="35"/>
+      <c r="B336" s="36"/>
+      <c r="C336" s="37"/>
+      <c r="D336" s="37"/>
+      <c r="E336" s="37"/>
+      <c r="F336" s="38"/>
     </row>
     <row r="337" spans="2:6" ht="87.75" customHeight="1" thickBot="1">
-      <c r="B337" s="36"/>
-      <c r="C337" s="37"/>
-      <c r="D337" s="37"/>
-      <c r="E337" s="37"/>
-      <c r="F337" s="38"/>
+      <c r="B337" s="39"/>
+      <c r="C337" s="40"/>
+      <c r="D337" s="40"/>
+      <c r="E337" s="40"/>
+      <c r="F337" s="41"/>
     </row>
     <row r="338" spans="2:6" ht="13.5" thickBot="1"/>
     <row r="339" spans="2:6" ht="21" thickBot="1">
-      <c r="B339" s="39" t="s">
+      <c r="B339" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="C339" s="39"/>
-      <c r="D339" s="39"/>
-      <c r="E339" s="39"/>
-      <c r="F339" s="39"/>
+      <c r="C339" s="42"/>
+      <c r="D339" s="42"/>
+      <c r="E339" s="42"/>
+      <c r="F339" s="42"/>
     </row>
     <row r="340" spans="2:6" ht="13.5" thickBot="1">
       <c r="B340" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C340" s="40" t="s">
+      <c r="C340" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="D340" s="41"/>
-      <c r="E340" s="41"/>
-      <c r="F340" s="42"/>
+      <c r="D340" s="44"/>
+      <c r="E340" s="44"/>
+      <c r="F340" s="45"/>
     </row>
     <row r="341" spans="2:6" ht="13.5" thickBot="1">
       <c r="B341" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C341" s="40" t="s">
+      <c r="C341" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="D341" s="41"/>
-      <c r="E341" s="41"/>
-      <c r="F341" s="42"/>
+      <c r="D341" s="44"/>
+      <c r="E341" s="44"/>
+      <c r="F341" s="45"/>
     </row>
     <row r="342" spans="2:6" ht="13.5" thickBot="1">
       <c r="B342" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C342" s="43" t="s">
+      <c r="C342" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="D342" s="44"/>
-      <c r="E342" s="44"/>
-      <c r="F342" s="45"/>
+      <c r="D342" s="47"/>
+      <c r="E342" s="47"/>
+      <c r="F342" s="48"/>
     </row>
     <row r="343" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
       <c r="B343" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C343" s="46" t="s">
+      <c r="C343" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D343" s="47"/>
-      <c r="E343" s="47"/>
-      <c r="F343" s="48"/>
+      <c r="D343" s="50"/>
+      <c r="E343" s="50"/>
+      <c r="F343" s="51"/>
     </row>
     <row r="344" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
       <c r="B344" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C344" s="49"/>
-      <c r="D344" s="50"/>
-      <c r="E344" s="50"/>
-      <c r="F344" s="51"/>
+      <c r="C344" s="52"/>
+      <c r="D344" s="53"/>
+      <c r="E344" s="53"/>
+      <c r="F344" s="54"/>
     </row>
     <row r="345" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B345" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C345" s="52" t="s">
+      <c r="C345" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D345" s="53"/>
-      <c r="E345" s="53"/>
-      <c r="F345" s="54"/>
+      <c r="D345" s="56"/>
+      <c r="E345" s="56"/>
+      <c r="F345" s="57"/>
     </row>
     <row r="346" spans="2:6" ht="42" customHeight="1" thickBot="1">
       <c r="B346" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C346" s="52" t="s">
+      <c r="C346" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D346" s="53"/>
-      <c r="E346" s="53"/>
-      <c r="F346" s="54"/>
+      <c r="D346" s="56"/>
+      <c r="E346" s="56"/>
+      <c r="F346" s="57"/>
     </row>
     <row r="347" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B347" s="52"/>
-      <c r="C347" s="53"/>
-      <c r="D347" s="53"/>
-      <c r="E347" s="53"/>
-      <c r="F347" s="54"/>
+      <c r="B347" s="55"/>
+      <c r="C347" s="56"/>
+      <c r="D347" s="56"/>
+      <c r="E347" s="56"/>
+      <c r="F347" s="57"/>
     </row>
     <row r="348" spans="2:6" ht="13.5" thickBot="1">
       <c r="B348" s="7" t="s">
@@ -11402,25 +11467,45 @@
       <c r="F349" s="26"/>
     </row>
     <row r="350" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B350" s="1"/>
-      <c r="C350" s="9"/>
-      <c r="D350" s="9"/>
-      <c r="E350" s="6"/>
-      <c r="F350" s="9"/>
+      <c r="B350" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C350" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D350" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E350" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F350" s="9" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="351" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B351" s="10"/>
-      <c r="C351" s="8"/>
-      <c r="D351" s="8"/>
-      <c r="E351" s="14"/>
-      <c r="F351" s="9"/>
+      <c r="B351" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C351" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D351" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E351" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="F351" s="9" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="352" spans="2:6" ht="14.25" thickBot="1">
-      <c r="B352" s="27"/>
-      <c r="C352" s="28"/>
-      <c r="D352" s="28"/>
-      <c r="E352" s="28"/>
-      <c r="F352" s="29"/>
+      <c r="B352" s="30"/>
+      <c r="C352" s="31"/>
+      <c r="D352" s="31"/>
+      <c r="E352" s="31"/>
+      <c r="F352" s="32"/>
     </row>
     <row r="353" spans="2:6" ht="13.5" thickBot="1">
       <c r="B353" s="24" t="s">
@@ -11465,7 +11550,7 @@
         <v>47</v>
       </c>
       <c r="D356" s="9" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
       <c r="E356" s="4"/>
       <c r="F356" s="9"/>
@@ -11508,126 +11593,401 @@
       <c r="F359" s="26"/>
     </row>
     <row r="360" spans="2:6">
-      <c r="B360" s="30" t="s">
+      <c r="B360" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="C360" s="31"/>
-      <c r="D360" s="31"/>
-      <c r="E360" s="31"/>
-      <c r="F360" s="32"/>
+      <c r="C360" s="34"/>
+      <c r="D360" s="34"/>
+      <c r="E360" s="34"/>
+      <c r="F360" s="35"/>
     </row>
     <row r="361" spans="2:6">
-      <c r="B361" s="33"/>
-      <c r="C361" s="34"/>
-      <c r="D361" s="34"/>
-      <c r="E361" s="34"/>
-      <c r="F361" s="35"/>
+      <c r="B361" s="36"/>
+      <c r="C361" s="37"/>
+      <c r="D361" s="37"/>
+      <c r="E361" s="37"/>
+      <c r="F361" s="38"/>
     </row>
     <row r="362" spans="2:6">
-      <c r="B362" s="33"/>
-      <c r="C362" s="34"/>
-      <c r="D362" s="34"/>
-      <c r="E362" s="34"/>
-      <c r="F362" s="35"/>
+      <c r="B362" s="36"/>
+      <c r="C362" s="37"/>
+      <c r="D362" s="37"/>
+      <c r="E362" s="37"/>
+      <c r="F362" s="38"/>
     </row>
     <row r="363" spans="2:6">
-      <c r="B363" s="33"/>
-      <c r="C363" s="34"/>
-      <c r="D363" s="34"/>
-      <c r="E363" s="34"/>
-      <c r="F363" s="35"/>
+      <c r="B363" s="36"/>
+      <c r="C363" s="37"/>
+      <c r="D363" s="37"/>
+      <c r="E363" s="37"/>
+      <c r="F363" s="38"/>
     </row>
     <row r="364" spans="2:6" ht="87.75" customHeight="1" thickBot="1">
-      <c r="B364" s="36"/>
-      <c r="C364" s="37"/>
-      <c r="D364" s="37"/>
-      <c r="E364" s="37"/>
-      <c r="F364" s="38"/>
+      <c r="B364" s="39"/>
+      <c r="C364" s="40"/>
+      <c r="D364" s="40"/>
+      <c r="E364" s="40"/>
+      <c r="F364" s="41"/>
+    </row>
+    <row r="366" spans="2:6" ht="13.5" thickBot="1"/>
+    <row r="367" spans="2:6" ht="21" thickBot="1">
+      <c r="B367" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="C367" s="42"/>
+      <c r="D367" s="42"/>
+      <c r="E367" s="42"/>
+      <c r="F367" s="42"/>
+    </row>
+    <row r="368" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B368" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C368" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="D368" s="44"/>
+      <c r="E368" s="44"/>
+      <c r="F368" s="45"/>
+    </row>
+    <row r="369" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B369" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C369" s="43" t="s">
+        <v>205</v>
+      </c>
+      <c r="D369" s="44"/>
+      <c r="E369" s="44"/>
+      <c r="F369" s="45"/>
+    </row>
+    <row r="370" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B370" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C370" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="D370" s="47"/>
+      <c r="E370" s="47"/>
+      <c r="F370" s="48"/>
+    </row>
+    <row r="371" spans="2:6" ht="12.75" customHeight="1" thickBot="1">
+      <c r="B371" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C371" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D371" s="50"/>
+      <c r="E371" s="50"/>
+      <c r="F371" s="51"/>
+    </row>
+    <row r="372" spans="2:6" ht="22.5" customHeight="1" thickBot="1">
+      <c r="B372" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C372" s="52"/>
+      <c r="D372" s="53"/>
+      <c r="E372" s="53"/>
+      <c r="F372" s="54"/>
+    </row>
+    <row r="373" spans="2:6" ht="42" customHeight="1" thickBot="1">
+      <c r="B373" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C373" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D373" s="56"/>
+      <c r="E373" s="56"/>
+      <c r="F373" s="57"/>
+    </row>
+    <row r="374" spans="2:6" ht="42" customHeight="1" thickBot="1">
+      <c r="B374" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C374" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D374" s="56"/>
+      <c r="E374" s="56"/>
+      <c r="F374" s="57"/>
+    </row>
+    <row r="375" spans="2:6" ht="44.25" customHeight="1" thickBot="1">
+      <c r="B375" s="55"/>
+      <c r="C375" s="56"/>
+      <c r="D375" s="56"/>
+      <c r="E375" s="56"/>
+      <c r="F375" s="57"/>
+    </row>
+    <row r="376" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B376" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C376" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D376" s="9"/>
+      <c r="E376" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F376" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="377" spans="2:6" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B377" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C377" s="25"/>
+      <c r="D377" s="25"/>
+      <c r="E377" s="25"/>
+      <c r="F377" s="26"/>
+    </row>
+    <row r="378" spans="2:6" ht="14.25" thickBot="1">
+      <c r="B378" s="1"/>
+      <c r="C378" s="9"/>
+      <c r="D378" s="9"/>
+      <c r="E378" s="6"/>
+      <c r="F378" s="9"/>
+    </row>
+    <row r="379" spans="2:6" ht="14.25" thickBot="1">
+      <c r="B379" s="10"/>
+      <c r="C379" s="8"/>
+      <c r="D379" s="8"/>
+      <c r="E379" s="14"/>
+      <c r="F379" s="9"/>
+    </row>
+    <row r="380" spans="2:6" ht="14.25" thickBot="1">
+      <c r="B380" s="30"/>
+      <c r="C380" s="31"/>
+      <c r="D380" s="31"/>
+      <c r="E380" s="31"/>
+      <c r="F380" s="32"/>
+    </row>
+    <row r="381" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B381" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C381" s="25"/>
+      <c r="D381" s="25"/>
+      <c r="E381" s="25"/>
+      <c r="F381" s="26"/>
+    </row>
+    <row r="382" spans="2:6" ht="14.25" thickBot="1">
+      <c r="B382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C382" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D382" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E382" s="4"/>
+      <c r="F382" s="4"/>
+    </row>
+    <row r="383" spans="2:6" ht="14.25" thickBot="1">
+      <c r="B383" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C383" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D383" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E383" s="4"/>
+      <c r="F383" s="4"/>
+    </row>
+    <row r="384" spans="2:6" ht="14.25" thickBot="1">
+      <c r="B384" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C384" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D384" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E384" s="4"/>
+      <c r="F384" s="9"/>
+    </row>
+    <row r="385" spans="2:6" ht="14.25" thickBot="1">
+      <c r="B385" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C385" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D385" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E385" s="11"/>
+      <c r="F385" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="386" spans="2:6" ht="14.25" thickBot="1">
+      <c r="B386" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C386" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D386" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E386" s="11"/>
+      <c r="F386" s="4"/>
+    </row>
+    <row r="387" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B387" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C387" s="25"/>
+      <c r="D387" s="25"/>
+      <c r="E387" s="25"/>
+      <c r="F387" s="26"/>
+    </row>
+    <row r="388" spans="2:6">
+      <c r="B388" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C388" s="34"/>
+      <c r="D388" s="34"/>
+      <c r="E388" s="34"/>
+      <c r="F388" s="35"/>
+    </row>
+    <row r="389" spans="2:6">
+      <c r="B389" s="36"/>
+      <c r="C389" s="37"/>
+      <c r="D389" s="37"/>
+      <c r="E389" s="37"/>
+      <c r="F389" s="38"/>
+    </row>
+    <row r="390" spans="2:6">
+      <c r="B390" s="36"/>
+      <c r="C390" s="37"/>
+      <c r="D390" s="37"/>
+      <c r="E390" s="37"/>
+      <c r="F390" s="38"/>
+    </row>
+    <row r="391" spans="2:6">
+      <c r="B391" s="36"/>
+      <c r="C391" s="37"/>
+      <c r="D391" s="37"/>
+      <c r="E391" s="37"/>
+      <c r="F391" s="38"/>
+    </row>
+    <row r="392" spans="2:6" ht="87.75" customHeight="1" thickBot="1">
+      <c r="B392" s="39"/>
+      <c r="C392" s="40"/>
+      <c r="D392" s="40"/>
+      <c r="E392" s="40"/>
+      <c r="F392" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="190">
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B252:F256"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="C226:F226"/>
-    <mergeCell ref="C227:F227"/>
-    <mergeCell ref="C228:F228"/>
-    <mergeCell ref="C229:F229"/>
-    <mergeCell ref="C230:F230"/>
-    <mergeCell ref="C231:F231"/>
-    <mergeCell ref="C232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F223"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="C199:F199"/>
-    <mergeCell ref="C200:F200"/>
-    <mergeCell ref="C201:F201"/>
-    <mergeCell ref="C202:F202"/>
-    <mergeCell ref="C203:F203"/>
-    <mergeCell ref="C204:F204"/>
-    <mergeCell ref="C205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B192:F196"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="C173:F173"/>
-    <mergeCell ref="C174:F174"/>
-    <mergeCell ref="C175:F175"/>
-    <mergeCell ref="C176:F176"/>
-    <mergeCell ref="C177:F177"/>
-    <mergeCell ref="C178:F178"/>
-    <mergeCell ref="C179:F179"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B166:F170"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="C150:F150"/>
-    <mergeCell ref="C151:F151"/>
-    <mergeCell ref="C152:F152"/>
-    <mergeCell ref="C153:F153"/>
-    <mergeCell ref="C154:F154"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F57"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="C122:F122"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F116"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="C121:F121"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
+  <mergeCells count="204">
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F392"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="C368:F368"/>
+    <mergeCell ref="C369:F369"/>
+    <mergeCell ref="C370:F370"/>
+    <mergeCell ref="C371:F371"/>
+    <mergeCell ref="C372:F372"/>
+    <mergeCell ref="C373:F373"/>
+    <mergeCell ref="C374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B360:F364"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="C340:F340"/>
+    <mergeCell ref="C341:F341"/>
+    <mergeCell ref="C342:F342"/>
+    <mergeCell ref="C343:F343"/>
+    <mergeCell ref="C344:F344"/>
+    <mergeCell ref="C345:F345"/>
+    <mergeCell ref="C346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="C286:F286"/>
+    <mergeCell ref="C287:F287"/>
+    <mergeCell ref="C288:F288"/>
+    <mergeCell ref="C289:F289"/>
+    <mergeCell ref="C290:F290"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B306:F310"/>
+    <mergeCell ref="C291:F291"/>
+    <mergeCell ref="C292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="C264:F264"/>
+    <mergeCell ref="C63:F63"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C66:F66"/>
+    <mergeCell ref="C67:F67"/>
+    <mergeCell ref="C68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="C265:F265"/>
+    <mergeCell ref="C266:F266"/>
+    <mergeCell ref="C95:F95"/>
+    <mergeCell ref="C96:F96"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="C261:F261"/>
+    <mergeCell ref="C262:F262"/>
+    <mergeCell ref="C263:F263"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B83:F87"/>
+    <mergeCell ref="C260:F260"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="C92:F92"/>
+    <mergeCell ref="C93:F93"/>
+    <mergeCell ref="C94:F94"/>
+    <mergeCell ref="C97:F97"/>
+    <mergeCell ref="C98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="C123:F123"/>
+    <mergeCell ref="C124:F124"/>
+    <mergeCell ref="C125:F125"/>
+    <mergeCell ref="C126:F126"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F143"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="C148:F148"/>
+    <mergeCell ref="C149:F149"/>
+    <mergeCell ref="C127:F127"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="B24:F24"/>
@@ -11652,90 +12012,88 @@
     <mergeCell ref="B272:F272"/>
     <mergeCell ref="B279:F283"/>
     <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B83:F87"/>
-    <mergeCell ref="C260:F260"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="C92:F92"/>
-    <mergeCell ref="C93:F93"/>
-    <mergeCell ref="C94:F94"/>
-    <mergeCell ref="C97:F97"/>
-    <mergeCell ref="C98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="C123:F123"/>
-    <mergeCell ref="C124:F124"/>
-    <mergeCell ref="C125:F125"/>
-    <mergeCell ref="C126:F126"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:F143"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="C148:F148"/>
-    <mergeCell ref="C149:F149"/>
-    <mergeCell ref="C127:F127"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="C264:F264"/>
-    <mergeCell ref="C63:F63"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C66:F66"/>
-    <mergeCell ref="C67:F67"/>
-    <mergeCell ref="C68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="C265:F265"/>
-    <mergeCell ref="C266:F266"/>
-    <mergeCell ref="C95:F95"/>
-    <mergeCell ref="C96:F96"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="C261:F261"/>
-    <mergeCell ref="C262:F262"/>
-    <mergeCell ref="C263:F263"/>
-    <mergeCell ref="C286:F286"/>
-    <mergeCell ref="C287:F287"/>
-    <mergeCell ref="C288:F288"/>
-    <mergeCell ref="C289:F289"/>
-    <mergeCell ref="C290:F290"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B306:F310"/>
-    <mergeCell ref="C291:F291"/>
-    <mergeCell ref="C292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B360:F364"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="C340:F340"/>
-    <mergeCell ref="C341:F341"/>
-    <mergeCell ref="C342:F342"/>
-    <mergeCell ref="C343:F343"/>
-    <mergeCell ref="C344:F344"/>
-    <mergeCell ref="C345:F345"/>
-    <mergeCell ref="C346:F346"/>
-    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F57"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C122:F122"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F116"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="C121:F121"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B166:F170"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="C150:F150"/>
+    <mergeCell ref="C151:F151"/>
+    <mergeCell ref="C152:F152"/>
+    <mergeCell ref="C153:F153"/>
+    <mergeCell ref="C154:F154"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B192:F196"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="C173:F173"/>
+    <mergeCell ref="C174:F174"/>
+    <mergeCell ref="C175:F175"/>
+    <mergeCell ref="C176:F176"/>
+    <mergeCell ref="C177:F177"/>
+    <mergeCell ref="C178:F178"/>
+    <mergeCell ref="C179:F179"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F223"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="C199:F199"/>
+    <mergeCell ref="C200:F200"/>
+    <mergeCell ref="C201:F201"/>
+    <mergeCell ref="C202:F202"/>
+    <mergeCell ref="C203:F203"/>
+    <mergeCell ref="C204:F204"/>
+    <mergeCell ref="C205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B252:F256"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="C226:F226"/>
+    <mergeCell ref="C227:F227"/>
+    <mergeCell ref="C228:F228"/>
+    <mergeCell ref="C229:F229"/>
+    <mergeCell ref="C230:F230"/>
+    <mergeCell ref="C231:F231"/>
+    <mergeCell ref="C232:F232"/>
+    <mergeCell ref="B233:F233"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
@@ -11765,9 +12123,11 @@
     <hyperlink ref="C227" r:id="rId24"/>
     <hyperlink ref="C200" r:id="rId25"/>
     <hyperlink ref="C199" r:id="rId26"/>
+    <hyperlink ref="C369" r:id="rId27"/>
+    <hyperlink ref="C368" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId27"/>
-  <drawing r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId29"/>
+  <drawing r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
recommend stocks by topic
</commit_message>
<xml_diff>
--- a/doc/Es搜索api接口_v2.xlsx
+++ b/doc/Es搜索api接口_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="25605" windowHeight="14205" tabRatio="632"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25605" windowHeight="14175" tabRatio="632"/>
   </bookViews>
   <sheets>
     <sheet name="V1搜索及推荐引擎提供接口列表" sheetId="9" r:id="rId1"/>
@@ -2023,10 +2023,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>http://192.168.100.12:8999/es/index/news</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>http://54.222.222.172:8999/es/index/news</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -5920,6 +5916,10 @@
   </si>
   <si>
     <t>默认为推荐&lt;=10个</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://192.168.100.12:8999/es/index/news</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -7901,8 +7901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B346" workbookViewId="0">
-      <selection activeCell="D356" sqref="D356"/>
+    <sheetView tabSelected="1" topLeftCell="B325" workbookViewId="0">
+      <selection activeCell="C372" sqref="C372:F372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -10169,7 +10169,7 @@
     </row>
     <row r="225" spans="2:6" ht="21" thickBot="1">
       <c r="B225" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C225" s="42"/>
       <c r="D225" s="42"/>
@@ -10181,7 +10181,7 @@
         <v>0</v>
       </c>
       <c r="C226" s="43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D226" s="44"/>
       <c r="E226" s="44"/>
@@ -10192,7 +10192,7 @@
         <v>81</v>
       </c>
       <c r="C227" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D227" s="47"/>
       <c r="E227" s="47"/>
@@ -10203,7 +10203,7 @@
         <v>83</v>
       </c>
       <c r="C228" s="46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D228" s="47"/>
       <c r="E228" s="47"/>
@@ -10234,7 +10234,7 @@
         <v>86</v>
       </c>
       <c r="C231" s="55" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D231" s="56"/>
       <c r="E231" s="56"/>
@@ -10284,7 +10284,7 @@
     </row>
     <row r="236" spans="2:6" ht="14.25" thickBot="1">
       <c r="B236" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C236" s="8" t="s">
         <v>88</v>
@@ -10296,109 +10296,109 @@
         <v>113</v>
       </c>
       <c r="F236" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="237" spans="2:6" ht="14.25" thickBot="1">
       <c r="B237" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C237" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="C237" s="8" t="s">
+      <c r="D237" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D237" s="8" t="s">
+      <c r="E237" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E237" s="11" t="s">
+      <c r="F237" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="F237" s="9" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="238" spans="2:6" ht="14.25" thickBot="1">
       <c r="B238" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C238" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="C238" s="8" t="s">
+      <c r="D238" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="D238" s="8" t="s">
+      <c r="E238" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F238" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="E238" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="F238" s="9" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="239" spans="2:6" ht="14.25" thickBot="1">
       <c r="B239" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C239" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="C239" s="8" t="s">
+      <c r="D239" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E239" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F239" s="9" t="s">
         <v>188</v>
-      </c>
-      <c r="D239" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E239" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="F239" s="9" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="240" spans="2:6" ht="14.25" thickBot="1">
       <c r="B240" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C240" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C240" s="8" t="s">
+      <c r="D240" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="D240" s="8" t="s">
-        <v>192</v>
-      </c>
       <c r="E240" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F240" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="241" spans="2:6" ht="14.25" thickBot="1">
       <c r="B241" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C241" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C241" s="8" t="s">
-        <v>194</v>
-      </c>
       <c r="D241" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E241" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F241" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="242" spans="2:6" ht="14.25" thickBot="1">
       <c r="B242" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C242" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="C242" s="8" t="s">
+      <c r="D242" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="D242" s="8" t="s">
+      <c r="E242" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="E242" s="11" t="s">
+      <c r="F242" s="9" t="s">
         <v>201</v>
-      </c>
-      <c r="F242" s="9" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="243" spans="2:6" ht="14.25" thickBot="1">
@@ -10506,7 +10506,7 @@
     </row>
     <row r="252" spans="2:6">
       <c r="B252" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C252" s="34"/>
       <c r="D252" s="34"/>
@@ -11365,7 +11365,7 @@
         <v>0</v>
       </c>
       <c r="C340" s="43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D340" s="44"/>
       <c r="E340" s="44"/>
@@ -11376,7 +11376,7 @@
         <v>58</v>
       </c>
       <c r="C341" s="43" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="D341" s="44"/>
       <c r="E341" s="44"/>
@@ -11468,36 +11468,36 @@
     </row>
     <row r="350" spans="2:6" ht="14.25" thickBot="1">
       <c r="B350" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C350" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="C350" s="9" t="s">
+      <c r="D350" s="9" t="s">
         <v>208</v>
-      </c>
-      <c r="D350" s="9" t="s">
-        <v>209</v>
       </c>
       <c r="E350" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F350" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="351" spans="2:6" ht="14.25" thickBot="1">
       <c r="B351" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C351" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C351" s="8" t="s">
+      <c r="D351" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="D351" s="8" t="s">
+      <c r="E351" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="E351" s="18" t="s">
+      <c r="F351" s="9" t="s">
         <v>214</v>
-      </c>
-      <c r="F351" s="9" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="352" spans="2:6" ht="14.25" thickBot="1">
@@ -11594,7 +11594,7 @@
     </row>
     <row r="360" spans="2:6">
       <c r="B360" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C360" s="34"/>
       <c r="D360" s="34"/>
@@ -11632,7 +11632,7 @@
     <row r="366" spans="2:6" ht="13.5" thickBot="1"/>
     <row r="367" spans="2:6" ht="21" thickBot="1">
       <c r="B367" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C367" s="42"/>
       <c r="D367" s="42"/>
@@ -11644,7 +11644,7 @@
         <v>0</v>
       </c>
       <c r="C368" s="43" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D368" s="44"/>
       <c r="E368" s="44"/>
@@ -11655,7 +11655,7 @@
         <v>58</v>
       </c>
       <c r="C369" s="43" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D369" s="44"/>
       <c r="E369" s="44"/>
@@ -11666,7 +11666,7 @@
         <v>15</v>
       </c>
       <c r="C370" s="46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D370" s="47"/>
       <c r="E370" s="47"/>
@@ -11853,7 +11853,7 @@
     </row>
     <row r="388" spans="2:6">
       <c r="B388" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C388" s="34"/>
       <c r="D388" s="34"/>

</xml_diff>